<commit_message>
skill full names added to PDP outputs and spreadsheets
</commit_message>
<xml_diff>
--- a/outputs/app-pdp-criteria-generator/buisness_analysis_academy_pdp.xlsx
+++ b/outputs/app-pdp-criteria-generator/buisness_analysis_academy_pdp.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>SkillCode</t>
   </si>
   <si>
+    <t>Skill Description</t>
+  </si>
+  <si>
     <t>SFIA Level</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t>REQM</t>
   </si>
   <si>
+    <t>Requirements definition and management</t>
+  </si>
+  <si>
     <t>Uses standard techniques to elicit, specify, and document requirements for simple subject areas with clearly-defined boundaries</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t>BPTS</t>
   </si>
   <si>
+    <t>Acceptance testing</t>
+  </si>
+  <si>
     <t>Assists in planning, preparing and executing acceptance tests for systems, products, business processes or services</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
     <t>DTAN</t>
   </si>
   <si>
+    <t>Data modelling and design</t>
+  </si>
+  <si>
     <t>Establishes, modifies or maintains simple data structures and associated components</t>
   </si>
   <si>
@@ -110,6 +122,9 @@
   </si>
   <si>
     <t>BSMO</t>
+  </si>
+  <si>
+    <t>Business modelling</t>
   </si>
   <si>
     <t>Understands the purpose and benefits of modelling</t>
@@ -444,328 +459,400 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="E6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
       <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
-        <v>13</v>
+      <c r="E8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
       </c>
       <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
+      <c r="E9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>16</v>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>17</v>
+      <c r="E11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
       <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
+      <c r="E13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
+      <c r="E14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
       </c>
       <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>22</v>
+      <c r="E15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>24</v>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
       </c>
       <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
-        <v>25</v>
+      <c r="E17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>27</v>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
-        <v>28</v>
+      <c r="E19" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>30</v>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21"/>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>32</v>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
       </c>
       <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
-        <v>33</v>
+      <c r="E23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
-        <v>34</v>
+      <c r="E24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
       </c>
       <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>35</v>
+      <c r="E25" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>